<commit_message>
correct joining component sample to floor plan and generated floods
</commit_message>
<xml_diff>
--- a/data/component_cost_lca_data.xlsx
+++ b/data/component_cost_lca_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\building_impact_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C8B4F0-AB36-4FD6-9CC5-377B2C7275A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448B364C-FE87-43FC-AD58-6B7EBC4997F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8264" uniqueCount="1781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8307" uniqueCount="1800">
   <si>
     <t>type</t>
   </si>
@@ -5385,10 +5385,67 @@
     <t>component_join</t>
   </si>
   <si>
-    <t>upstairs a</t>
-  </si>
-  <si>
-    <t>downstairs b</t>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
   </si>
 </sst>
 </file>
@@ -28640,10 +28697,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A623DF7-8824-47EF-81D7-78EB44C59BE6}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -28673,7 +28730,7 @@
         <v>1766</v>
       </c>
       <c r="C2" t="s">
-        <v>1779</v>
+        <v>1797</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -28687,9 +28744,23 @@
         <v>1767</v>
       </c>
       <c r="C3" t="s">
-        <v>1780</v>
+        <v>1798</v>
       </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
     </row>
@@ -28700,10 +28771,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FC1A9E-6FD9-4DE2-9760-917D84C43308}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B2:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -28778,6 +28849,166 @@
       </c>
       <c r="B9" t="s">
         <v>1772</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>898</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>